<commit_message>
Completed Assert Datasets Equal command and tested
</commit_message>
<xml_diff>
--- a/docs/test_workbook_feature8.xlsx
+++ b/docs/test_workbook_feature8.xlsx
@@ -1,27 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnoto\Documents\_Other\Source\Repos\dataunit\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FF9D3FA-3927-47E3-9C27-E76281653B3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CB902E-6E40-47B6-8FE0-BC8EE8E7C0C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1395" windowWidth="28110" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-1395" windowWidth="28110" windowHeight="16440" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
     <sheet name="Test Commands" sheetId="2" r:id="rId2"/>
-    <sheet name="Test_Dataset_1" sheetId="8" r:id="rId3"/>
-    <sheet name="Settings" sheetId="4" r:id="rId4"/>
+    <sheet name="Settings" sheetId="4" r:id="rId3"/>
+    <sheet name="Diet_Log_1" sheetId="8" r:id="rId4"/>
     <sheet name="_commands" sheetId="6" state="hidden" r:id="rId5"/>
     <sheet name="_command_parameters" sheetId="7" state="hidden" r:id="rId6"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Test Commands'!$A$1:$M$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Test Commands'!$A$1:$M$12</definedName>
     <definedName name="CommandType">_commands!$A$2:$A$13</definedName>
     <definedName name="TestParameters">#REF!</definedName>
   </definedNames>
@@ -46,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="150">
   <si>
     <t>Active</t>
   </si>
@@ -282,13 +285,43 @@
     <t>Test Commands</t>
   </si>
   <si>
-    <t>Some Command</t>
-  </si>
-  <si>
-    <t>Diet_Log_Id</t>
-  </si>
-  <si>
-    <t>Profile_Id</t>
+    <t>${DB_CONNECTION}</t>
+  </si>
+  <si>
+    <t>DB_CONNECTION</t>
+  </si>
+  <si>
+    <t>Database connection string</t>
+  </si>
+  <si>
+    <t>sql_statement</t>
+  </si>
+  <si>
+    <t>connection_string</t>
+  </si>
+  <si>
+    <t>Execute query and return result</t>
+  </si>
+  <si>
+    <t>Compare expected and actual results</t>
+  </si>
+  <si>
+    <t>expected_dataset</t>
+  </si>
+  <si>
+    <t>expected_dataset_type</t>
+  </si>
+  <si>
+    <t>Worksheet</t>
+  </si>
+  <si>
+    <t>actual_dataset</t>
+  </si>
+  <si>
+    <t>actual_dataset_type</t>
+  </si>
+  <si>
+    <t>Resultset</t>
   </si>
   <si>
     <t>Log_Date</t>
@@ -306,52 +339,166 @@
     <t>Quantity</t>
   </si>
   <si>
+    <t>First_Name</t>
+  </si>
+  <si>
+    <t>Last_Name</t>
+  </si>
+  <si>
+    <t>Breakfast</t>
+  </si>
+  <si>
+    <t>Glazed Donut</t>
+  </si>
+  <si>
+    <t>Christel</t>
+  </si>
+  <si>
+    <t>Russen</t>
+  </si>
+  <si>
+    <t>Coke (12 oz.)</t>
+  </si>
+  <si>
+    <t>Lunch</t>
+  </si>
+  <si>
+    <t>Ham Sandwich</t>
+  </si>
+  <si>
+    <t>Potato Chips</t>
+  </si>
+  <si>
+    <t>Chocolate Chip Cookie</t>
+  </si>
+  <si>
     <t>Snack</t>
   </si>
   <si>
-    <t>Fiber Bar</t>
-  </si>
-  <si>
-    <t>Carrots and Dip</t>
-  </si>
-  <si>
-    <t>Spaghetti and Meatballs</t>
-  </si>
-  <si>
-    <t>DB_CONNECTION</t>
-  </si>
-  <si>
-    <t>Database connection string</t>
-  </si>
-  <si>
-    <t>2018-03-15</t>
-  </si>
-  <si>
-    <t>DRIVER={SQL Server};SERVER=localhost;DATABASE=MyFitBot;Trusted_Connection=yes;</t>
-  </si>
-  <si>
-    <t>Test_Dataset_1</t>
-  </si>
-  <si>
-    <t>expected_dataset</t>
-  </si>
-  <si>
-    <t>expected_dataset_type</t>
-  </si>
-  <si>
-    <t>Worksheet</t>
-  </si>
-  <si>
-    <t>actual_dataset</t>
-  </si>
-  <si>
-    <t>actual_dataset_type</t>
-  </si>
-  <si>
-    <t>Resultset</t>
-  </si>
-  <si>
-    <t>${resultset_1}</t>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Coffee</t>
+  </si>
+  <si>
+    <t>Greek Salad</t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>Dinner</t>
+  </si>
+  <si>
+    <t>Steak (8 oz.)</t>
+  </si>
+  <si>
+    <t>Mashed Potatoes (1 cup)</t>
+  </si>
+  <si>
+    <t>Green Beans (1 cup)</t>
+  </si>
+  <si>
+    <t>Red Wine (5 oz.)</t>
+  </si>
+  <si>
+    <t>Grilled Salmon (6 oz.)</t>
+  </si>
+  <si>
+    <t>Quinoa (.75 cup)</t>
+  </si>
+  <si>
+    <t>Granola Bar</t>
+  </si>
+  <si>
+    <t>190</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>290</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>390</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>680</t>
+  </si>
+  <si>
+    <t>215</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>340</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>Diet_Log_1</t>
+  </si>
+  <si>
+    <t>diet_log</t>
+  </si>
+  <si>
+    <t>SELECT * FROM dbo.Diet_Log_Profile_Test</t>
+  </si>
+  <si>
+    <t>result_variable_name</t>
+  </si>
+  <si>
+    <t>DRIVER={SQL Server};SERVER=localhost;DATABASE=MyFitBot;UID=SA;PWD=dataunitSQL2020!;</t>
+  </si>
+  <si>
+    <t>2018-02-15 08:30:18</t>
+  </si>
+  <si>
+    <t>2018-02-15 12:30:35</t>
+  </si>
+  <si>
+    <t>2018-02-15 15:12:19</t>
+  </si>
+  <si>
+    <t>2018-02-16 08:00:45</t>
+  </si>
+  <si>
+    <t>2018-02-16 12:14:19</t>
+  </si>
+  <si>
+    <t>2018-02-16 14:08:34</t>
+  </si>
+  <si>
+    <t>2018-02-15 18:30:57</t>
+  </si>
+  <si>
+    <t>2018-02-16 18:08:34</t>
+  </si>
+  <si>
+    <t>2018-02-16 21:03:16</t>
   </si>
 </sst>
 </file>
@@ -498,6 +645,228 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Tests"/>
+      <sheetName val="Test Commands"/>
+      <sheetName val="Settings"/>
+      <sheetName val="_commands"/>
+      <sheetName val="_command_parameters"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4">
+        <row r="2">
+          <cell r="C2" t="str">
+            <v>Execute SQL-1</v>
+          </cell>
+          <cell r="D2" t="str">
+            <v>SQL</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="C3" t="str">
+            <v>Execute SQL-2</v>
+          </cell>
+          <cell r="D3" t="str">
+            <v>Connection</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="C4" t="str">
+            <v>Execute SQL With Resultset-1</v>
+          </cell>
+          <cell r="D4" t="str">
+            <v>SQL</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="C5" t="str">
+            <v>Execute SQL With Resultset-2</v>
+          </cell>
+          <cell r="D5" t="str">
+            <v>Connection</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="C6" t="str">
+            <v>Execute SQL With Resultset-3</v>
+          </cell>
+          <cell r="D6" t="str">
+            <v>ResultVariableName</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7" t="str">
+            <v>Execute Shell Command-1</v>
+          </cell>
+          <cell r="D7" t="str">
+            <v>Command</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8" t="str">
+            <v>Load Sheet to Table-1</v>
+          </cell>
+          <cell r="D8" t="str">
+            <v>Sheet Name</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="C9" t="str">
+            <v>Load Sheet to Table-2</v>
+          </cell>
+          <cell r="D9" t="str">
+            <v>Table Name</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="C10" t="str">
+            <v>Load Sheet to Table-3</v>
+          </cell>
+          <cell r="D10" t="str">
+            <v>Connection</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11" t="str">
+            <v>Load Sheet to Table-4</v>
+          </cell>
+          <cell r="D11" t="str">
+            <v>Truncate Table</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12" t="str">
+            <v>Save Sheet to File-1</v>
+          </cell>
+          <cell r="D12" t="str">
+            <v>Sheet Name</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="C13" t="str">
+            <v>Save Sheet to File-2</v>
+          </cell>
+          <cell r="D13" t="str">
+            <v>File Path Name</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="C14" t="str">
+            <v>Save Sheet to File-3</v>
+          </cell>
+          <cell r="D14" t="str">
+            <v>File Format</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="C15" t="str">
+            <v>Assert Datasets Equal-1</v>
+          </cell>
+          <cell r="D15" t="str">
+            <v>Expected Dataset</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="C16" t="str">
+            <v>Assert Datasets Equal-2</v>
+          </cell>
+          <cell r="D16" t="str">
+            <v>Expected Dataset Type</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="C17" t="str">
+            <v>Assert Datasets Equal-3</v>
+          </cell>
+          <cell r="D17" t="str">
+            <v>Actual Dataset</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="C18" t="str">
+            <v>Assert Datasets Equal-4</v>
+          </cell>
+          <cell r="D18" t="str">
+            <v>Actual Dataset Type</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="C19" t="str">
+            <v>Assert SQL Records Returned-1</v>
+          </cell>
+          <cell r="D19" t="str">
+            <v>SQL</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="C20" t="str">
+            <v>Assert SQL Records Returned-2</v>
+          </cell>
+          <cell r="D20" t="str">
+            <v>Connection</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="C21" t="str">
+            <v>Assert SQL No Records Returned-1</v>
+          </cell>
+          <cell r="D21" t="str">
+            <v>SQL</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="C22" t="str">
+            <v>Assert SQL No Records Returned-2</v>
+          </cell>
+          <cell r="D22" t="str">
+            <v>Connection</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="C23" t="str">
+            <v>Assert SQL Single Value Returned-1</v>
+          </cell>
+          <cell r="D23" t="str">
+            <v>SQL</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="C24" t="str">
+            <v>Assert SQL Single Value Returned-2</v>
+          </cell>
+          <cell r="D24" t="str">
+            <v>Connection</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="C25" t="str">
+            <v>Assert Last Return Code Equal-1</v>
+          </cell>
+          <cell r="D25" t="str">
+            <v>Expected Return Code</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="C26" t="str">
+            <v>Assert Last Return Code Not Equal-1</v>
+          </cell>
+          <cell r="D26" t="str">
+            <v>Expected Return Code</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -765,21 +1134,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" style="5" customWidth="1"/>
     <col min="2" max="2" width="9.5" style="5" customWidth="1"/>
-    <col min="3" max="3" width="35.375" style="12" customWidth="1"/>
-    <col min="4" max="4" width="30.125" style="12" customWidth="1"/>
-    <col min="5" max="16384" width="10.875" style="12"/>
+    <col min="3" max="3" width="35.33203125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="30.08203125" style="12" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>58</v>
       </c>
@@ -793,7 +1162,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>74</v>
       </c>
@@ -807,109 +1176,109 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="9"/>
       <c r="B3" s="8"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="9"/>
@@ -928,32 +1297,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.5" style="5" customWidth="1"/>
     <col min="2" max="2" width="30.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="17.375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="12" customWidth="1"/>
     <col min="5" max="5" width="33.5" style="13" customWidth="1"/>
-    <col min="6" max="6" width="18.625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="19.375" style="12" customWidth="1"/>
+    <col min="6" max="6" width="18.58203125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" style="12" customWidth="1"/>
     <col min="8" max="8" width="19.5" style="12" customWidth="1"/>
-    <col min="9" max="9" width="18.375" style="12" customWidth="1"/>
-    <col min="10" max="10" width="19.375" style="12" customWidth="1"/>
-    <col min="11" max="11" width="21.375" style="12" customWidth="1"/>
-    <col min="12" max="12" width="19.375" style="12" customWidth="1"/>
-    <col min="13" max="13" width="21.375" style="12" customWidth="1"/>
-    <col min="14" max="16384" width="10.875" style="12"/>
+    <col min="9" max="9" width="18.33203125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="21.33203125" style="12" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="12" customWidth="1"/>
+    <col min="13" max="13" width="21.33203125" style="12" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -994,77 +1363,83 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>75</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="H2" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J2" s="10"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="10" t="str">
+        <f>IF($C2="","",IF(ISNA(VLOOKUP($C2&amp;"-"&amp;MID($L$1,11,1),[1]_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C2&amp;"-"&amp;MID($L$1,11,1),[1]_command_parameters!$C$2:$D$26,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="M2" s="9"/>
+    </row>
+    <row r="3" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="L2" s="10" t="str">
-        <f>IF($C2="","",IF(ISNA(VLOOKUP($C2&amp;"-"&amp;MID($L$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C2&amp;"-"&amp;MID($L$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
-        <v/>
-      </c>
-      <c r="M2" s="9"/>
-    </row>
-    <row r="3" spans="1:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="10" t="str">
-        <f>IF($C3="","",IF(ISNA(VLOOKUP($C3&amp;"-"&amp;MID($D$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C3&amp;"-"&amp;MID($D$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
-        <v/>
-      </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="10" t="str">
-        <f>IF($C3="","",IF(ISNA(VLOOKUP($C3&amp;"-"&amp;MID($F$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C3&amp;"-"&amp;MID($F$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
-        <v/>
-      </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="10" t="str">
-        <f>IF($C3="","",IF(ISNA(VLOOKUP($C3&amp;"-"&amp;MID($H$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C3&amp;"-"&amp;MID($H$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
-        <v/>
-      </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10" t="str">
-        <f>IF($C3="","",IF(ISNA(VLOOKUP($C3&amp;"-"&amp;MID($J$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C3&amp;"-"&amp;MID($J$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
-        <v/>
-      </c>
-      <c r="K3" s="9"/>
+      <c r="D3" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="L3" s="10" t="str">
         <f>IF($C3="","",IF(ISNA(VLOOKUP($C3&amp;"-"&amp;MID($L$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C3&amp;"-"&amp;MID($L$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
         <v/>
       </c>
       <c r="M3" s="9"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -1077,7 +1452,7 @@
         <f>IF($C4="","",IF(ISNA(VLOOKUP($C4&amp;"-"&amp;MID($F$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C4&amp;"-"&amp;MID($F$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
         <v/>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="11"/>
       <c r="H4" s="10" t="str">
         <f>IF($C4="","",IF(ISNA(VLOOKUP($C4&amp;"-"&amp;MID($H$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C4&amp;"-"&amp;MID($H$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
         <v/>
@@ -1094,7 +1469,7 @@
       </c>
       <c r="M4" s="9"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -1124,7 +1499,7 @@
       </c>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -1154,7 +1529,7 @@
       </c>
       <c r="M6" s="9"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -1167,7 +1542,7 @@
         <f>IF($C7="","",IF(ISNA(VLOOKUP($C7&amp;"-"&amp;MID($F$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C7&amp;"-"&amp;MID($F$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
         <v/>
       </c>
-      <c r="G7" s="11"/>
+      <c r="G7" s="9"/>
       <c r="H7" s="10" t="str">
         <f>IF($C7="","",IF(ISNA(VLOOKUP($C7&amp;"-"&amp;MID($H$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C7&amp;"-"&amp;MID($H$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
         <v/>
@@ -1184,7 +1559,7 @@
       </c>
       <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -1197,7 +1572,7 @@
         <f>IF($C8="","",IF(ISNA(VLOOKUP($C8&amp;"-"&amp;MID($F$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C8&amp;"-"&amp;MID($F$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
         <v/>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="11"/>
       <c r="H8" s="10" t="str">
         <f>IF($C8="","",IF(ISNA(VLOOKUP($C8&amp;"-"&amp;MID($H$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C8&amp;"-"&amp;MID($H$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
         <v/>
@@ -1214,7 +1589,7 @@
       </c>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -1244,7 +1619,7 @@
       </c>
       <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -1274,7 +1649,7 @@
       </c>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -1304,7 +1679,7 @@
       </c>
       <c r="M11" s="9"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -1317,7 +1692,7 @@
         <f>IF($C12="","",IF(ISNA(VLOOKUP($C12&amp;"-"&amp;MID($F$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C12&amp;"-"&amp;MID($F$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
         <v/>
       </c>
-      <c r="G12" s="11"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="10" t="str">
         <f>IF($C12="","",IF(ISNA(VLOOKUP($C12&amp;"-"&amp;MID($H$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C12&amp;"-"&amp;MID($H$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
         <v/>
@@ -1334,7 +1709,7 @@
       </c>
       <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="1:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -1364,7 +1739,7 @@
       </c>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -1377,7 +1752,7 @@
         <f>IF($C14="","",IF(ISNA(VLOOKUP($C14&amp;"-"&amp;MID($F$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C14&amp;"-"&amp;MID($F$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
         <v/>
       </c>
-      <c r="G14" s="9"/>
+      <c r="G14" s="11"/>
       <c r="H14" s="10" t="str">
         <f>IF($C14="","",IF(ISNA(VLOOKUP($C14&amp;"-"&amp;MID($H$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C14&amp;"-"&amp;MID($H$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
         <v/>
@@ -1394,7 +1769,7 @@
       </c>
       <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -1424,7 +1799,7 @@
       </c>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -1454,7 +1829,7 @@
       </c>
       <c r="M16" s="9"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -1467,7 +1842,7 @@
         <f>IF($C17="","",IF(ISNA(VLOOKUP($C17&amp;"-"&amp;MID($F$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C17&amp;"-"&amp;MID($F$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
         <v/>
       </c>
-      <c r="G17" s="11"/>
+      <c r="G17" s="9"/>
       <c r="H17" s="10" t="str">
         <f>IF($C17="","",IF(ISNA(VLOOKUP($C17&amp;"-"&amp;MID($H$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C17&amp;"-"&amp;MID($H$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
         <v/>
@@ -1484,7 +1859,7 @@
       </c>
       <c r="M17" s="9"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -1497,7 +1872,7 @@
         <f>IF($C18="","",IF(ISNA(VLOOKUP($C18&amp;"-"&amp;MID($F$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C18&amp;"-"&amp;MID($F$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
         <v/>
       </c>
-      <c r="G18" s="9"/>
+      <c r="G18" s="11"/>
       <c r="H18" s="10" t="str">
         <f>IF($C18="","",IF(ISNA(VLOOKUP($C18&amp;"-"&amp;MID($H$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C18&amp;"-"&amp;MID($H$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
         <v/>
@@ -1514,7 +1889,7 @@
       </c>
       <c r="M18" s="9"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="8"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -1544,7 +1919,7 @@
       </c>
       <c r="M19" s="9"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -1574,7 +1949,7 @@
       </c>
       <c r="M20" s="9"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -1604,13 +1979,43 @@
       </c>
       <c r="M21" s="9"/>
     </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="10" t="str">
+        <f>IF($C22="","",IF(ISNA(VLOOKUP($C22&amp;"-"&amp;MID($D$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C22&amp;"-"&amp;MID($D$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="10" t="str">
+        <f>IF($C22="","",IF(ISNA(VLOOKUP($C22&amp;"-"&amp;MID($F$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C22&amp;"-"&amp;MID($F$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="10" t="str">
+        <f>IF($C22="","",IF(ISNA(VLOOKUP($C22&amp;"-"&amp;MID($H$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C22&amp;"-"&amp;MID($H$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="I22" s="9"/>
+      <c r="J22" s="10" t="str">
+        <f>IF($C22="","",IF(ISNA(VLOOKUP($C22&amp;"-"&amp;MID($J$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C22&amp;"-"&amp;MID($J$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="K22" s="9"/>
+      <c r="L22" s="10" t="str">
+        <f>IF($C22="","",IF(ISNA(VLOOKUP($C22&amp;"-"&amp;MID($L$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)),"",VLOOKUP($C22&amp;"-"&amp;MID($L$1,11,1),_command_parameters!$C$2:$D$26,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="M22" s="9"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M11" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:M12" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2 A4:A12 A14:A1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A15:A1048576 A5:A13 A2:A3" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 C3:C1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>CommandType</formula1>
     </dataValidation>
   </dataValidations>
@@ -1621,138 +2026,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>41</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2">
-        <v>140</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>42</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>43</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4">
-        <v>800</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.58203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="76.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.875" style="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -1763,203 +2052,203 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1970,8 +2259,539 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A888A69A-925C-4A9A-9F5B-58BFB464FF77}">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="16"/>
+    <col min="3" max="3" width="29.33203125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="15.08203125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="16"/>
+    <col min="6" max="6" width="10.4140625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="11.08203125" style="16" customWidth="1"/>
+    <col min="8" max="16384" width="8.6640625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1979,14 +2799,14 @@
       <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="33.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="65.875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.875" style="1"/>
+    <col min="2" max="2" width="65.83203125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>62</v>
       </c>
@@ -1994,7 +2814,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2002,7 +2822,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>68</v>
       </c>
@@ -2010,7 +2830,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2018,7 +2838,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -2026,7 +2846,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -2034,7 +2854,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -2042,7 +2862,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -2050,7 +2870,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -2058,7 +2878,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -2066,7 +2886,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -2074,7 +2894,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -2089,24 +2909,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="33" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.08203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="50.625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.875" style="1"/>
+    <col min="5" max="5" width="50.58203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>62</v>
       </c>
@@ -2123,7 +2943,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2141,7 +2961,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2159,7 +2979,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>68</v>
       </c>
@@ -2177,7 +2997,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>68</v>
       </c>
@@ -2195,7 +3015,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>68</v>
       </c>
@@ -2213,7 +3033,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -2231,7 +3051,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -2249,7 +3069,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -2267,7 +3087,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -2285,7 +3105,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -2303,7 +3123,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -2321,7 +3141,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
@@ -2339,7 +3159,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -2357,7 +3177,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2375,7 +3195,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -2393,7 +3213,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -2411,7 +3231,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
@@ -2429,7 +3249,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -2447,7 +3267,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -2465,7 +3285,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -2483,7 +3303,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -2501,7 +3321,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -2519,7 +3339,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -2537,7 +3357,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
@@ -2555,7 +3375,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
@@ -2575,7 +3395,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:C1048576" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:C1048576" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>CommandType</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>